<commit_message>
wip new install mod logic
</commit_message>
<xml_diff>
--- a/AdvanceTools/Tools/ThaiStorybook/storybook.xlsx
+++ b/AdvanceTools/Tools/ThaiStorybook/storybook.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="1000" firstSheet="10" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="1000" firstSheet="55" activeTab="61"/>
   </bookViews>
   <sheets>
     <sheet name="fb_1a_tr" sheetId="1" r:id="rId1"/>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1270" uniqueCount="739">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1271" uniqueCount="740">
   <si>
     <t>D:\Project\mod\ThaiStoryBook\modThaiStoryBook\files\movies\cutscenes\finalboards\subs\fb_1a_tr.subs</t>
   </si>
@@ -2302,6 +2302,9 @@
   </si>
   <si>
     <t>เกิดอะไรขึ้นกับ Ciri? เป็นสิ่งที่บอกได้ยาก ตั้งแต่เหตุการณ์ที่ Undvik ก็ยังไม่มีใครได้พบเห็นนางอีกเลย</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ciri ไม่ได้พบ Elven mage แต่พวก Wild Hunt ต่างหากที่ได้เจอ ดูเหมือนว่าบริวารของพวกผีร้ายได้ล้ำหน้า Geralt ไป 1 ก้าว Witcher รู้สึกเหมือนหมดหนทางแล้ว กระทั่ง Keira ได้บอกเขาถึงเบาะแสใหม่ นั่นคือ The Crones of Crookback Bog </t>
   </si>
 </sst>
 </file>
@@ -2346,7 +2349,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
@@ -2355,6 +2358,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3323,7 +3327,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
@@ -7974,8 +7978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8031,10 +8035,13 @@
       <c r="C5" s="1" t="s">
         <v>471</v>
       </c>
+      <c r="D5" s="6" t="s">
+        <v>739</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>